<commit_message>
capital of china is beijing
</commit_message>
<xml_diff>
--- a/PythonPals/python_questions_capitals.xlsx
+++ b/PythonPals/python_questions_capitals.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Sheamus\School\Senior\Python\PythonPals\PythonPals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/srivastavar_ufl_edu/Documents/2020 Fall/CIS4930/PythonPals/PythonPals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F47EC58-7D7D-435E-9DD9-2BAC5441DEC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{7F47EC58-7D7D-435E-9DD9-2BAC5441DEC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9CA2B4AF-463F-4893-B892-B5D456458902}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" xr2:uid="{84F58A44-D10C-4044-AB84-18E9D6FE800B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{84F58A44-D10C-4044-AB84-18E9D6FE800B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -714,12 +714,12 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I21"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -748,7 +748,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -775,7 +775,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -802,7 +802,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -829,7 +829,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -856,7 +856,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -883,7 +883,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -895,7 +895,7 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
         <v>37</v>
@@ -910,7 +910,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -937,7 +937,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -964,7 +964,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -991,7 +991,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>

</xml_diff>